<commit_message>
lagt til felt for ikke voksne personer
også endret controller route slik at den gir mer mening nå. Endret fra
"Application" til "API"
</commit_message>
<xml_diff>
--- a/timetable-prototype.xlsx
+++ b/timetable-prototype.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dokumenty\Github\Webapplikasjoner-Oppgave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE90B37-711E-4130-B50B-49BF45AD1604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B560FE-9EA3-4875-884B-232FD76E23FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="540" windowWidth="27900" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28275" yWindow="915" windowWidth="27900" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Oslo</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>300kr</t>
+  </si>
+  <si>
+    <t>ikke voksen pris</t>
+  </si>
+  <si>
+    <t>350kr</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,10 +427,12 @@
     <col min="3" max="3" width="44.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -441,13 +449,16 @@
         <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -464,13 +475,16 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -487,9 +501,12 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new routes, prices and times for departure
</commit_message>
<xml_diff>
--- a/timetable-prototype.xlsx
+++ b/timetable-prototype.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dokumenty\Github\Webapplikasjoner-Oppgave\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blerton\source\repos\karol-121\Webapplikasjoner-Oppgave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B560FE-9EA3-4875-884B-232FD76E23FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99E63E4-589E-466E-90C3-CE28CD340C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28275" yWindow="915" windowWidth="27900" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24615" yWindow="2235" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Oslo</t>
   </si>
@@ -48,18 +48,12 @@
     <t>mandag, onsdag, fredag</t>
   </si>
   <si>
-    <t>9.00, 17.00</t>
-  </si>
-  <si>
     <t>Bergen</t>
   </si>
   <si>
     <t>torsdag</t>
   </si>
   <si>
-    <t>10.00</t>
-  </si>
-  <si>
     <t>Enkelperson pris</t>
   </si>
   <si>
@@ -69,31 +63,82 @@
     <t>motorvogn pris</t>
   </si>
   <si>
-    <t>500kr</t>
-  </si>
-  <si>
-    <t>100kr</t>
-  </si>
-  <si>
-    <t>200kr</t>
-  </si>
-  <si>
-    <t>400kr</t>
-  </si>
-  <si>
-    <t>300kr</t>
-  </si>
-  <si>
     <t>ikke voksen pris</t>
   </si>
   <si>
-    <t>350kr</t>
+    <t>Oslo/Norge</t>
+  </si>
+  <si>
+    <t>Hirtshals/Danmark</t>
+  </si>
+  <si>
+    <t>Larvik/Norge</t>
+  </si>
+  <si>
+    <t>København/Danmark</t>
+  </si>
+  <si>
+    <t>Bodø/Norge</t>
+  </si>
+  <si>
+    <t>Moskenes/Norge</t>
+  </si>
+  <si>
+    <t>Sandefjord/Norge</t>
+  </si>
+  <si>
+    <t>Strømstad/Sverige</t>
+  </si>
+  <si>
+    <t>Stavanger/Norge</t>
+  </si>
+  <si>
+    <t>Bergen/Norge</t>
+  </si>
+  <si>
+    <t>Kiel/Tyskland</t>
+  </si>
+  <si>
+    <t>mandag, tirsdag, onsdag, torsdag, fredag</t>
+  </si>
+  <si>
+    <t>07:00, 15:00</t>
+  </si>
+  <si>
+    <t>tirsdag, torsdag, lørdag</t>
+  </si>
+  <si>
+    <t>mandag, onsdag, fredag, søndag</t>
+  </si>
+  <si>
+    <t>09:00, 16:00</t>
+  </si>
+  <si>
+    <t>mandag, torsdag, lørdag</t>
+  </si>
+  <si>
+    <t>12:00, 22:00</t>
+  </si>
+  <si>
+    <t>fredag, lørdag, søndag, mandag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mandag, onsdag, fredag </t>
+  </si>
+  <si>
+    <t>08:00, 17:00</t>
+  </si>
+  <si>
+    <t>09:00, 17:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="[$NOK]\ #,##0.00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -132,9 +177,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,24 +467,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -446,19 +499,19 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -468,46 +521,202 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2">
+        <v>500</v>
+      </c>
+      <c r="F2" s="2">
+        <v>400</v>
+      </c>
+      <c r="G2" s="2">
+        <v>100</v>
+      </c>
+      <c r="H2" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E3" s="2">
+        <v>400</v>
+      </c>
+      <c r="F3" s="2">
+        <v>350</v>
+      </c>
+      <c r="G3" s="2">
+        <v>100</v>
+      </c>
+      <c r="H3" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="2">
+        <v>549</v>
+      </c>
+      <c r="F9" s="2">
+        <v>399</v>
+      </c>
+      <c r="G9" s="2">
+        <v>100</v>
+      </c>
+      <c r="H9" s="2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E10" s="2">
+        <v>499</v>
+      </c>
+      <c r="F10" s="2">
+        <v>299</v>
+      </c>
+      <c r="G10" s="2">
+        <v>100</v>
+      </c>
+      <c r="H10" s="2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="2">
+        <v>749</v>
+      </c>
+      <c r="F11" s="2">
+        <v>299</v>
+      </c>
+      <c r="G11" s="2">
+        <v>100</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="2">
+        <v>399</v>
+      </c>
+      <c r="F12" s="2">
+        <v>299</v>
+      </c>
+      <c r="G12" s="2">
+        <v>100</v>
+      </c>
+      <c r="H12" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2">
+        <v>499</v>
+      </c>
+      <c r="F13" s="2">
+        <v>349</v>
+      </c>
+      <c r="G13" s="2">
+        <v>100</v>
+      </c>
+      <c r="H13" s="2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E14" s="2">
+        <v>399</v>
+      </c>
+      <c r="F14" s="2">
+        <v>349</v>
+      </c>
+      <c r="G14" s="2">
+        <v>100</v>
+      </c>
+      <c r="H14" s="2">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lagt til nye forslag på den nye tidstabel (excel)
</commit_message>
<xml_diff>
--- a/timetable-prototype.xlsx
+++ b/timetable-prototype.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blerton\source\repos\karol-121\Webapplikasjoner-Oppgave\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dokumenty\Github\Webapplikasjoner-Oppgave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206A4B84-589B-4900-885F-6E590DE39562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AFCD75-4995-417F-BBE1-C155F04D67B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="1320" windowWidth="25050" windowHeight="13395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
   <si>
     <t>Oslo</t>
   </si>
@@ -99,9 +99,6 @@
     <t xml:space="preserve">mandag, onsdag, fredag </t>
   </si>
   <si>
-    <t>08:00, 17:00</t>
-  </si>
-  <si>
     <t>NOK 549.00</t>
   </si>
   <si>
@@ -184,6 +181,42 @@
   </si>
   <si>
     <t>tirsdag, torsdag, lørdag</t>
+  </si>
+  <si>
+    <t>Sandefjord</t>
+  </si>
+  <si>
+    <t>Strømstad</t>
+  </si>
+  <si>
+    <t>Stavanger</t>
+  </si>
+  <si>
+    <t>Kiel</t>
+  </si>
+  <si>
+    <t>tirsdag, torsdag</t>
+  </si>
+  <si>
+    <t>lørdag</t>
+  </si>
+  <si>
+    <t>8.00, 17.00</t>
+  </si>
+  <si>
+    <t>9.00, 18.00</t>
+  </si>
+  <si>
+    <t>8.00, 15.00</t>
+  </si>
+  <si>
+    <t>NOK 200.00</t>
+  </si>
+  <si>
+    <t>NOK 449.00</t>
+  </si>
+  <si>
+    <t>8.00, 16.00</t>
   </si>
 </sst>
 </file>
@@ -231,7 +264,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,24 +545,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="44.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -555,7 +589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -565,7 +599,7 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
@@ -581,7 +615,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -591,7 +625,7 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
@@ -607,7 +641,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -617,150 +657,267 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2">
+        <v>0.33353206018518522</v>
+      </c>
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>26</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>27</v>
       </c>
-      <c r="H6" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
       </c>
       <c r="D7" s="2">
         <v>0.58333333333333337</v>
       </c>
       <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="B11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
       </c>
       <c r="D11" s="2">
         <v>0.58333333333333337</v>
       </c>
       <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
         <v>26</v>
       </c>
-      <c r="F11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" t="s">
         <v>27</v>
       </c>
-      <c r="H11" t="s">
-        <v>33</v>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modifisert dbinit etter den nye excel forslag
</commit_message>
<xml_diff>
--- a/timetable-prototype.xlsx
+++ b/timetable-prototype.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dokumenty\Github\Webapplikasjoner-Oppgave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AFCD75-4995-417F-BBE1-C155F04D67B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E27931-CC16-4838-8C3A-C30DCEC4FF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="1320" windowWidth="25050" windowHeight="13395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26010" yWindow="1440" windowWidth="25050" windowHeight="13395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t>Oslo</t>
   </si>
@@ -204,9 +204,6 @@
     <t>8.00, 17.00</t>
   </si>
   <si>
-    <t>9.00, 18.00</t>
-  </si>
-  <si>
     <t>8.00, 15.00</t>
   </si>
   <si>
@@ -216,7 +213,7 @@
     <t>NOK 449.00</t>
   </si>
   <si>
-    <t>8.00, 16.00</t>
+    <t>maks plasser</t>
   </si>
 </sst>
 </file>
@@ -545,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +560,7 @@
     <col min="8" max="8" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -588,8 +585,11 @@
       <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -615,7 +615,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -641,13 +641,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -673,7 +673,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -699,7 +699,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -725,7 +725,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -751,7 +751,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -777,7 +777,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -803,13 +803,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -823,7 +823,7 @@
         <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14" t="s">
         <v>32</v>
@@ -834,19 +834,20 @@
       <c r="H14" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
       <c r="B15" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -857,7 +858,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
         <v>24</v>
@@ -871,19 +872,19 @@
       <c r="H17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>54</v>
       </c>
-      <c r="D18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -906,18 +907,18 @@
         <v>26</v>
       </c>
       <c r="H20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="I20">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>55</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
-      </c>
-      <c r="D21" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>